<commit_message>
Added Waitaki flow data
</commit_message>
<xml_diff>
--- a/data/File_Navigation.xlsx
+++ b/data/File_Navigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6cb6b6143dae0d7/Documents/R/browser/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55981CAD-75CA-4DD0-930B-F99D7644EF7D}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{318D132F-50D9-4C45-921A-202068296CA0}"/>
   <bookViews>
-    <workbookView xWindow="8724" yWindow="0" windowWidth="16116" windowHeight="11844" activeTab="1" xr2:uid="{52163122-39DA-4AC1-834B-3EB0B25A5BD9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{52163122-39DA-4AC1-834B-3EB0B25A5BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>Climate</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>New Zealand Stations Metadata</t>
+  </si>
+  <si>
+    <t>Waitaki Flow Dataset</t>
+  </si>
+  <si>
+    <t>Waitaki_flow.xlsx</t>
   </si>
 </sst>
 </file>
@@ -622,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF6C410-5600-45F5-A753-74F7DE3CBA5F}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1017,6 +1023,17 @@
         <v>44</v>
       </c>
     </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added logan hydrology data
</commit_message>
<xml_diff>
--- a/data/File_Navigation.xlsx
+++ b/data/File_Navigation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6cb6b6143dae0d7/Documents/R/browser/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{318D132F-50D9-4C45-921A-202068296CA0}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42EF544E-BD54-43C9-8C49-416AE001FFF1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{52163122-39DA-4AC1-834B-3EB0B25A5BD9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>Climate</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>Waitaki_flow.xlsx</t>
+  </si>
+  <si>
+    <t>Logan Hydrology Data</t>
+  </si>
+  <si>
+    <t>logan_hydrology_final.xlsx</t>
   </si>
 </sst>
 </file>
@@ -628,10 +634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF6C410-5600-45F5-A753-74F7DE3CBA5F}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -986,19 +992,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20">
-        <v>-44.2</v>
-      </c>
-      <c r="E20">
-        <v>170.5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1006,10 +1006,16 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <v>-44.2</v>
+      </c>
+      <c r="E21">
+        <v>170.5</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1017,10 +1023,10 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1028,9 +1034,20 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>